<commit_message>
working w/ customized document and json
</commit_message>
<xml_diff>
--- a/TestCustom.xlsx
+++ b/TestCustom.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RFonseca\workRepos\AsposeAPI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C095C00-E28A-48B1-9741-DCA7C261938A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="-1"/>
+    <workbookView xWindow="10020" yWindow="4905" windowWidth="22110" windowHeight="12495" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart" sheetId="4" r:id="rId7"/>
-    <sheet name="Data_Cells" sheetId="6" r:id="rId9"/>
+    <sheet name="Chart" sheetId="5" r:id="rId5"/>
+    <sheet name="Data_Cells" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>PositionId</t>
   </si>
@@ -64,16 +71,13 @@
     <t>Description Three</t>
   </si>
   <si>
-    <t>Junk</t>
-  </si>
-  <si>
-    <t>junk</t>
+    <t>testy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -88,7 +92,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -111,6 +115,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -423,7 +435,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -548,291 +560,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <a:themeElements>
     <a:clrScheme name="">
       <a:dk1>
@@ -884,7 +613,7 @@
         <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -951,263 +680,36 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" tabSelected="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>1123456</v>
-      </c>
-      <c r="B2" s="0">
-        <v>2123456</v>
-      </c>
-      <c r="C2" s="0">
-        <v>3123456</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="0">
-        <v>43466</v>
-      </c>
-      <c r="G2" s="0">
-        <v>43467</v>
-      </c>
-      <c r="H2" s="0">
-        <v>0</v>
-      </c>
-      <c r="I2" s="0">
-        <v>60000</v>
-      </c>
-      <c r="J2" s="0">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0">
-        <v>2123456</v>
-      </c>
-      <c r="B3" s="0">
-        <v>2123456</v>
-      </c>
-      <c r="C3" s="0">
-        <v>3123456</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="0">
-        <v>43467</v>
-      </c>
-      <c r="G3" s="0">
-        <v>43468</v>
-      </c>
-      <c r="H3" s="0">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0">
-        <v>60000</v>
-      </c>
-      <c r="J3" s="0">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0">
-        <v>3123456</v>
-      </c>
-      <c r="B4" s="0">
-        <v>32123456</v>
-      </c>
-      <c r="C4" s="0">
-        <v>3123456</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="0">
-        <v>43468</v>
-      </c>
-      <c r="G4" s="0">
-        <v>43469</v>
-      </c>
-      <c r="H4" s="0">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0">
-        <v>60000</v>
-      </c>
-      <c r="J4" s="0">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0">
-        <v>4123456</v>
-      </c>
-      <c r="B5" s="0">
-        <v>4123456</v>
-      </c>
-      <c r="C5" s="0">
-        <v>3123456</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="0">
-        <v>43469</v>
-      </c>
-      <c r="G5" s="0">
-        <v>43470</v>
-      </c>
-      <c r="H5" s="0">
-        <v>0</v>
-      </c>
-      <c r="I5" s="0">
-        <v>60000</v>
-      </c>
-      <c r="J5" s="0">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0">
-        <v>123456</v>
-      </c>
-      <c r="B6" s="0">
-        <v>2123456</v>
-      </c>
-      <c r="C6" s="0">
-        <v>3123456</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="0">
-        <v>43471</v>
-      </c>
-      <c r="G6" s="0">
-        <v>43472</v>
-      </c>
-      <c r="H6" s="0">
-        <v>0</v>
-      </c>
-      <c r="I6" s="0">
-        <v>60000</v>
-      </c>
-      <c r="J6" s="0">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="0">
-        <v>342342</v>
-      </c>
-      <c r="B7" s="0">
-        <v>43242</v>
-      </c>
-      <c r="C7" s="0">
-        <v>43234</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="0">
-        <v>344</v>
-      </c>
-      <c r="G7" s="0">
-        <v>4342</v>
-      </c>
-      <c r="H7" s="0">
-        <v>434</v>
-      </c>
-      <c r="I7" s="0">
-        <v>4342</v>
-      </c>
-      <c r="J7" s="0">
-        <v>4343</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="0" gridLines="0" gridLinesSet="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <sheetData/>
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" tabSelected="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1239,7 +741,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="0">
         <v>1123456</v>
       </c>
@@ -1271,7 +773,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="0">
         <v>2123456</v>
       </c>
@@ -1303,7 +805,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="0">
         <v>3123456</v>
       </c>
@@ -1335,7 +837,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="0">
         <v>4123456</v>
       </c>
@@ -1367,7 +869,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="0">
         <v>123456</v>
       </c>
@@ -1401,40 +903,38 @@
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" s="0">
-        <v>342342</v>
+        <v>43242342</v>
       </c>
       <c r="B7" s="0">
-        <v>43242</v>
+        <v>42343</v>
       </c>
       <c r="C7" s="0">
-        <v>43234</v>
+        <v>4234234</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="0">
-        <v>344</v>
+        <v>42342</v>
       </c>
       <c r="G7" s="0">
-        <v>4342</v>
+        <v>42343</v>
       </c>
       <c r="H7" s="0">
-        <v>434</v>
+        <v>4</v>
       </c>
       <c r="I7" s="0">
-        <v>4342</v>
+        <v>423423</v>
       </c>
       <c r="J7" s="0">
-        <v>4343</v>
+        <v>42423</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0" gridLinesSet="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>